<commit_message>
corrigindo interface e adicionando deepseek
</commit_message>
<xml_diff>
--- a/Estudos/Interface/Usuario.xlsx
+++ b/Estudos/Interface/Usuario.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -570,6 +570,131 @@
         <v>1.45</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Charles Ferreira</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="D6" t="n">
+        <v>4.24</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.77</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1.43</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>testando</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>2.42</v>
+      </c>
+      <c r="C7" t="n">
+        <v>5</v>
+      </c>
+      <c r="D7" t="n">
+        <v>4.95</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="F7" t="n">
+        <v>2.56</v>
+      </c>
+      <c r="G7" t="n">
+        <v>3.34</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.91</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1.05</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.8100000000000001</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.8100000000000001</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>deepseek</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="C10" t="n">
+        <v>5</v>
+      </c>
+      <c r="D10" t="n">
+        <v>4.75</v>
+      </c>
+      <c r="E10" t="n">
+        <v>3.39</v>
+      </c>
+      <c r="F10" t="n">
+        <v>1.78</v>
+      </c>
+      <c r="G10" t="n">
+        <v>3.88</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
adicionando versão final da interface e corrigindo endereços de carregamento dos modelos
</commit_message>
<xml_diff>
--- a/Estudos/Interface/Usuario.xlsx
+++ b/Estudos/Interface/Usuario.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -548,101 +548,69 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Usuario teste 1</t>
+          <t>Murilo Silva</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2.12</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0.87</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.76</v>
-      </c>
-      <c r="E5" t="n">
-        <v>1.65</v>
-      </c>
-      <c r="F5" t="n">
-        <v>1.83</v>
-      </c>
+        <v>3.19</v>
+      </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
       <c r="G5" t="n">
-        <v>1.45</v>
+        <v>3.19</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Charles Ferreira</t>
+          <t>Murilo Silva</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.78</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0.5600000000000001</v>
-      </c>
-      <c r="D6" t="n">
-        <v>4.24</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.77</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0.8</v>
-      </c>
+        <v>2.9</v>
+      </c>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
       <c r="G6" t="n">
-        <v>1.43</v>
+        <v>2.9</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>testando</t>
+          <t>Murilo Silva</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2.42</v>
-      </c>
-      <c r="C7" t="n">
-        <v>5</v>
-      </c>
-      <c r="D7" t="n">
-        <v>4.95</v>
-      </c>
-      <c r="E7" t="n">
-        <v>1.75</v>
-      </c>
-      <c r="F7" t="n">
-        <v>2.56</v>
-      </c>
+        <v>2.14</v>
+      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
       <c r="G7" t="n">
-        <v>3.34</v>
+        <v>2.14</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>b</t>
+          <t>teste</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.91</v>
-      </c>
-      <c r="C8" t="n">
-        <v>0.68</v>
-      </c>
-      <c r="D8" t="n">
-        <v>1.05</v>
-      </c>
-      <c r="E8" t="n">
-        <v>1.01</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0.8100000000000001</v>
-      </c>
+        <v>0.52</v>
+      </c>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
       <c r="G8" t="n">
-        <v>0.89</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="9">
@@ -652,47 +620,268 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.44</v>
-      </c>
-      <c r="C9" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0.63</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0.76</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0.8100000000000001</v>
-      </c>
+        <v>0.59</v>
+      </c>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
       <c r="G9" t="n">
-        <v>0.75</v>
+        <v>0.59</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>deepseek</t>
+          <t>b</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="C10" t="n">
-        <v>5</v>
-      </c>
-      <c r="D10" t="n">
-        <v>4.75</v>
-      </c>
-      <c r="E10" t="n">
-        <v>3.39</v>
-      </c>
-      <c r="F10" t="n">
-        <v>1.78</v>
-      </c>
+        <v>1.99</v>
+      </c>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
       <c r="G10" t="n">
-        <v>3.88</v>
+        <v>1.99</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Charles</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>1.36</v>
+      </c>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="n">
+        <v>1.36</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Murilo</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>3.45</v>
+      </c>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="n">
+        <v>3.45</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Murilo alves</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>2.79</v>
+      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="n">
+        <v>2.79</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>gabriel</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="C14" t="n">
+        <v>2.71</v>
+      </c>
+      <c r="D14" t="n">
+        <v>2.62</v>
+      </c>
+      <c r="E14" t="n">
+        <v>2.75</v>
+      </c>
+      <c r="F14" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="G14" t="n">
+        <v>2.68</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>testando</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="n">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Destro</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>4.49</v>
+      </c>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="n">
+        <v>4.49</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>t</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>1.91</v>
+      </c>
+      <c r="C17" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="D17" t="n">
+        <v>3.28</v>
+      </c>
+      <c r="E17" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="F17" t="n">
+        <v>2.38</v>
+      </c>
+      <c r="G17" t="n">
+        <v>2.12</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>1.36</v>
+      </c>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="n">
+        <v>1.36</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>2.25</v>
+      </c>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="n">
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>2.11</v>
+      </c>
+      <c r="C20" t="inlineStr"/>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="n">
+        <v>2.11</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>1.36</v>
+      </c>
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="n">
+        <v>1.36</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="C22" t="inlineStr"/>
+      <c r="D22" t="inlineStr"/>
+      <c r="E22" t="inlineStr"/>
+      <c r="F22" t="inlineStr"/>
+      <c r="G22" t="n">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>testando0000</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>1.21</v>
+      </c>
+      <c r="C23" t="inlineStr"/>
+      <c r="D23" t="inlineStr"/>
+      <c r="E23" t="inlineStr"/>
+      <c r="F23" t="inlineStr"/>
+      <c r="G23" t="n">
+        <v>1.21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adicionando analise das correcoes
</commit_message>
<xml_diff>
--- a/Estudos/Interface/Usuario.xlsx
+++ b/Estudos/Interface/Usuario.xlsx
@@ -548,408 +548,392 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Murilo Silva</t>
+          <t>Charles</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3.19</v>
+        <v>5</v>
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="n">
-        <v>3.19</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Murilo Silva</t>
+          <t>Matheus</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2.9</v>
+        <v>4.03</v>
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="n">
-        <v>2.9</v>
+        <v>4.03</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Murilo Silva</t>
+          <t>Murilo</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2.14</v>
+        <v>3.61</v>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="n">
-        <v>2.14</v>
+        <v>3.61</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>teste</t>
+          <t>Teste1</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.52</v>
+        <v>3.24</v>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="n">
-        <v>0.52</v>
+        <v>3.24</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>teste2</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.59</v>
+        <v>4.38</v>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="n">
-        <v>0.59</v>
+        <v>4.38</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>b</t>
+          <t>teste</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1.99</v>
+        <v>5</v>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="n">
-        <v>1.99</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Charles</t>
+          <t>teste</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1.36</v>
+        <v>3.96</v>
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="n">
-        <v>1.36</v>
+        <v>3.96</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Murilo</t>
+          <t>uy</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>3.45</v>
+        <v>1.64</v>
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="n">
-        <v>3.45</v>
+        <v>1.64</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Murilo alves</t>
+          <t>teste</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>2.79</v>
+        <v>3.59</v>
       </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="n">
-        <v>2.79</v>
+        <v>3.59</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>gabriel</t>
+          <t>Guilherme Ormond</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>2.7</v>
-      </c>
-      <c r="C14" t="n">
-        <v>2.71</v>
-      </c>
-      <c r="D14" t="n">
-        <v>2.62</v>
-      </c>
-      <c r="E14" t="n">
-        <v>2.75</v>
-      </c>
-      <c r="F14" t="n">
-        <v>2.6</v>
-      </c>
+        <v>3.57</v>
+      </c>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
       <c r="G14" t="n">
-        <v>2.68</v>
+        <v>3.57</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>testando</t>
+          <t>teste</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.52</v>
+        <v>3.67</v>
       </c>
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="n">
-        <v>0.52</v>
+        <v>3.67</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Destro</t>
+          <t>danilo</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>4.49</v>
+        <v>3.97</v>
       </c>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="n">
-        <v>4.49</v>
+        <v>3.97</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>t</t>
+          <t>Murilo</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1.91</v>
-      </c>
-      <c r="C17" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="D17" t="n">
-        <v>3.28</v>
-      </c>
-      <c r="E17" t="n">
-        <v>1.14</v>
-      </c>
-      <c r="F17" t="n">
-        <v>2.38</v>
-      </c>
+        <v>4.55</v>
+      </c>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr"/>
       <c r="G17" t="n">
-        <v>2.12</v>
+        <v>4.55</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>Ricardo Scopel</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>1.36</v>
+        <v>3.73</v>
       </c>
       <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="n">
-        <v>1.36</v>
+        <v>3.73</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>Gustavo Bertoluzzi Cardoso</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>2.25</v>
+        <v>3.72</v>
       </c>
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr"/>
       <c r="G19" t="n">
-        <v>2.25</v>
+        <v>3.72</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>Gustavo Flores</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>2.11</v>
+        <v>3.38</v>
       </c>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="n">
-        <v>2.11</v>
+        <v>3.38</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>Luana</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1.36</v>
+        <v>3.56</v>
       </c>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="n">
-        <v>1.36</v>
+        <v>3.56</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>Rafael Testa</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.99</v>
+        <v>4.49</v>
       </c>
       <c r="C22" t="inlineStr"/>
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr"/>
       <c r="G22" t="n">
-        <v>0.99</v>
+        <v>4.49</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>testando0000</t>
+          <t>Rafael</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>1.21</v>
+        <v>4.48</v>
       </c>
       <c r="C23" t="inlineStr"/>
       <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr"/>
       <c r="G23" t="n">
-        <v>1.21</v>
+        <v>4.48</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>asd</t>
+          <t>teste4</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>3.35</v>
+        <v>3.75</v>
       </c>
       <c r="C24" t="inlineStr"/>
       <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr"/>
       <c r="G24" t="n">
-        <v>3.35</v>
+        <v>3.75</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>asd</t>
+          <t>joao</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>3.42</v>
+        <v>3.66</v>
       </c>
       <c r="C25" t="inlineStr"/>
       <c r="D25" t="inlineStr"/>
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr"/>
       <c r="G25" t="n">
-        <v>3.42</v>
+        <v>3.66</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>aaaaaa</t>
+          <t>Gabriel</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>2.14</v>
+        <v>4.03</v>
       </c>
       <c r="C26" t="inlineStr"/>
       <c r="D26" t="inlineStr"/>
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr"/>
       <c r="G26" t="n">
-        <v>2.14</v>
+        <v>4.03</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>asdasd</t>
+          <t>Teste5</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.9</v>
+        <v>3.9</v>
       </c>
       <c r="C27" t="inlineStr"/>
       <c r="D27" t="inlineStr"/>
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr"/>
       <c r="G27" t="n">
-        <v>0.9</v>
+        <v>3.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>